<commit_message>
frontend table example, key fix
</commit_message>
<xml_diff>
--- a/dataSource/tableFromJS.xlsx
+++ b/dataSource/tableFromJS.xlsx
@@ -2121,13 +2121,13 @@
     <t>descDe</t>
   </si>
   <si>
-    <t>frontenendDe</t>
-  </si>
-  <si>
     <t>descEn</t>
   </si>
   <si>
     <t>frontendEd</t>
+  </si>
+  <si>
+    <t>frontendDe</t>
   </si>
 </sst>
 </file>
@@ -2469,12 +2469,13 @@
   <dimension ref="A1:F203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="109" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2488,13 +2489,13 @@
         <v>700</v>
       </c>
       <c r="D1" t="s">
+        <v>703</v>
+      </c>
+      <c r="E1" t="s">
         <v>701</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>702</v>
-      </c>
-      <c r="F1" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>